<commit_message>
Interfaces changes to get the people's names fron the data base and Telegram message added
</commit_message>
<xml_diff>
--- a/src/my_code/datos_empleados.xlsx
+++ b/src/my_code/datos_empleados.xlsx
@@ -20,21 +20,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
-  <si>
-    <t xml:space="preserve">NOMBRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEPARTAMENTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_DEP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POSICION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pablo Juan</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+  <si>
+    <t xml:space="preserve">Nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Departamento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID_Departamento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID_Telegram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Posicion_Base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Posicion_Recogida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iván José Aparicio</t>
   </si>
   <si>
     <t xml:space="preserve">Departamento de Imagen y Sonido</t>
@@ -55,10 +61,13 @@
     <t xml:space="preserve">d</t>
   </si>
   <si>
-    <t xml:space="preserve">-5.00_0.5_1.57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-15.00_3.00_1.57</t>
+    <t xml:space="preserve">972080220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-9.00_-2.0_2.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4.50_3.50_0.0</t>
   </si>
   <si>
     <t xml:space="preserve">Martín García</t>
@@ -104,7 +113,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -125,6 +134,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -176,16 +192,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -206,17 +230,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -232,95 +258,122 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>7</v>
+        <v>21</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
+        <v>27</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" display="972080220"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>